<commit_message>
fixed scale on idt table
</commit_message>
<xml_diff>
--- a/A3_test_oligos.xlsx
+++ b/A3_test_oligos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michaelvolk\Documents\repos\grna_scrape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED4465A-AEDB-4A7A-A181-B4DB6D880DEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2EC02D-2E39-40BE-931E-8F5D2F471093}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="5430" windowWidth="19440" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -34,12 +34,6 @@
     <t>Purification</t>
   </si>
   <si>
-    <t>YNL268W_sgtF_URA3F</t>
-  </si>
-  <si>
-    <t>YNL268W_sgtR_URA3R</t>
-  </si>
-  <si>
     <t>YOR128C_sgtR</t>
   </si>
   <si>
@@ -74,6 +68,15 @@
   </si>
   <si>
     <t>AAAGGTCTCAAAACCTAGACACAGGGTAATAACTGATATAATTAAATTGAAGCTC</t>
+  </si>
+  <si>
+    <t>100nm</t>
+  </si>
+  <si>
+    <t>YNL268W_sgtR_URA3</t>
+  </si>
+  <si>
+    <t>YNL268W_sgtF_URA3</t>
   </si>
 </sst>
 </file>
@@ -515,7 +518,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -542,86 +545,86 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>